<commit_message>
11/13/2019 5:38 pm Ran some stuff and got good results
</commit_message>
<xml_diff>
--- a/RESULTS_IEEE30_MainModelsTest_100Epochs.xlsx
+++ b/RESULTS_IEEE30_MainModelsTest_100Epochs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Sparsity</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Model 6</t>
+  </si>
+  <si>
+    <t>Model 7</t>
   </si>
 </sst>
 </file>
@@ -392,13 +395,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,8 +423,11 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -429,25 +435,28 @@
         <v>0.1</v>
       </c>
       <c r="C2">
-        <v>0.7080000042915344</v>
+        <v>0.6200000047683716</v>
       </c>
       <c r="D2">
-        <v>0.8845000267028809</v>
+        <v>0.859499990940094</v>
       </c>
       <c r="E2">
-        <v>0.9054999947547913</v>
+        <v>0.7789999842643738</v>
       </c>
       <c r="F2">
-        <v>0.8985000252723694</v>
+        <v>0.7595000267028809</v>
       </c>
       <c r="G2">
-        <v>0.6934999823570251</v>
+        <v>0.7925000190734863</v>
       </c>
       <c r="H2">
-        <v>0.734499990940094</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>0.8355000019073486</v>
+      </c>
+      <c r="I2">
+        <v>0.6769999861717224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -455,25 +464,28 @@
         <v>0.2</v>
       </c>
       <c r="C3">
-        <v>0.8309999704360962</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="D3">
-        <v>0.9825000166893005</v>
+        <v>0.9775000214576721</v>
       </c>
       <c r="E3">
-        <v>0.9865000247955322</v>
+        <v>0.9704999923706055</v>
       </c>
       <c r="F3">
-        <v>0.9944999814033508</v>
+        <v>0.9635000228881836</v>
       </c>
       <c r="G3">
-        <v>0.9574999809265137</v>
+        <v>0.9695000052452087</v>
       </c>
       <c r="H3">
-        <v>0.9635000228881836</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>0.9789999723434448</v>
+      </c>
+      <c r="I3">
+        <v>0.9359999895095825</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -481,25 +493,28 @@
         <v>0.3</v>
       </c>
       <c r="C4">
-        <v>0.9114999771118164</v>
+        <v>0.878000020980835</v>
       </c>
       <c r="D4">
-        <v>0.9940000176429749</v>
+        <v>0.9950000047683716</v>
       </c>
       <c r="E4">
-        <v>0.9980000257492065</v>
+        <v>0.9909999966621399</v>
       </c>
       <c r="F4">
-        <v>0.9984999895095825</v>
+        <v>0.9835000038146973</v>
       </c>
       <c r="G4">
-        <v>0.9735000133514404</v>
+        <v>0.9850000143051147</v>
       </c>
       <c r="H4">
-        <v>0.9725000262260437</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>0.9955000281333923</v>
+      </c>
+      <c r="I4">
+        <v>0.9620000123977661</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -507,25 +522,28 @@
         <v>0.4</v>
       </c>
       <c r="C5">
-        <v>0.8169999718666077</v>
+        <v>0.8859999775886536</v>
       </c>
       <c r="D5">
+        <v>0.9965000152587891</v>
+      </c>
+      <c r="E5">
+        <v>0.987500011920929</v>
+      </c>
+      <c r="F5">
+        <v>0.9879999756813049</v>
+      </c>
+      <c r="G5">
+        <v>0.9890000224113464</v>
+      </c>
+      <c r="H5">
         <v>0.9934999942779541</v>
       </c>
-      <c r="E5">
-        <v>0.9980000257492065</v>
-      </c>
-      <c r="F5">
-        <v>0.9984999895095825</v>
-      </c>
-      <c r="G5">
-        <v>0.9815000295639038</v>
-      </c>
-      <c r="H5">
-        <v>0.9745000004768372</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <v>0.9670000076293945</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -533,25 +551,28 @@
         <v>0.5</v>
       </c>
       <c r="C6">
-        <v>0.9670000076293945</v>
+        <v>0.9925000071525574</v>
       </c>
       <c r="D6">
-        <v>0.8404999971389771</v>
+        <v>0.5109999775886536</v>
       </c>
       <c r="E6">
-        <v>0.5044999718666077</v>
+        <v>0.7269999980926514</v>
       </c>
       <c r="F6">
-        <v>0.515500009059906</v>
+        <v>0.815500020980835</v>
       </c>
       <c r="G6">
-        <v>0.5674999952316284</v>
+        <v>0.5870000123977661</v>
       </c>
       <c r="H6">
-        <v>0.7009999752044678</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>0.6104999780654907</v>
+      </c>
+      <c r="I6">
+        <v>0.9980000257492065</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -559,25 +580,28 @@
         <v>0.6</v>
       </c>
       <c r="C7">
-        <v>0.9704999923706055</v>
+        <v>0.9940000176429749</v>
       </c>
       <c r="D7">
-        <v>0.9990000128746033</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0.9994999766349792</v>
       </c>
       <c r="G7">
-        <v>0.9994999766349792</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>0.9994999766349792</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0.9975000023841858</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -585,25 +609,28 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="C8">
-        <v>0.9894999861717224</v>
+        <v>0.9994999766349792</v>
       </c>
       <c r="D8">
-        <v>0.9955000281333923</v>
+        <v>0.9980000257492065</v>
       </c>
       <c r="E8">
-        <v>0.8410000205039978</v>
+        <v>0.9984999895095825</v>
       </c>
       <c r="F8">
+        <v>0.9994999766349792</v>
+      </c>
+      <c r="G8">
         <v>0.9980000257492065</v>
       </c>
-      <c r="G8">
-        <v>0.9990000128746033</v>
-      </c>
       <c r="H8">
-        <v>0.9984999895095825</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>0.9944999814033508</v>
+      </c>
+      <c r="I8">
+        <v>0.9994999766349792</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -611,25 +638,28 @@
         <v>0.8</v>
       </c>
       <c r="C9">
-        <v>0.9754999876022339</v>
+        <v>0.9994999766349792</v>
       </c>
       <c r="D9">
-        <v>0.9965000152587891</v>
+        <v>0.9990000128746033</v>
       </c>
       <c r="E9">
-        <v>0.9850000143051147</v>
+        <v>0.9975000023841858</v>
       </c>
       <c r="F9">
-        <v>0.9714999794960022</v>
+        <v>0.9994999766349792</v>
       </c>
       <c r="G9">
-        <v>0.9955000281333923</v>
+        <v>0.9975000023841858</v>
       </c>
       <c r="H9">
         <v>0.9975000023841858</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <v>0.9994999766349792</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -637,25 +667,28 @@
         <v>0.9</v>
       </c>
       <c r="C10">
-        <v>0.9860000014305115</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>0.9994999766349792</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>0.9994999766349792</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>0.9994999766349792</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>0.9994999766349792</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -663,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0.9940000176429749</v>
+        <v>0.9994999766349792</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -678,6 +711,9 @@
         <v>1</v>
       </c>
       <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
         <v>1</v>
       </c>
     </row>

</xml_diff>